<commit_message>
update data keuangan daurah
</commit_message>
<xml_diff>
--- a/Daurah Masyaikh Asrama Haji.xlsx
+++ b/Daurah Masyaikh Asrama Haji.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumen Pribadi\Ma'had\mds\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Mutasi Kas" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Chek" sheetId="3" r:id="rId3"/>
     <sheet name="Detail" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="130">
   <si>
     <t>Mutasi Kas Daurah Masyaikh di Surakarta</t>
   </si>
@@ -401,20 +406,23 @@
   </si>
   <si>
     <t>Amplop hansip + Pinjam lampu</t>
+  </si>
+  <si>
+    <t>Transfer ke sie kebersihan</t>
+  </si>
+  <si>
+    <t>Biaya Transfer ke sie kebersihan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,150 +462,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,7 +477,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399914548173467"/>
+        <fgColor theme="4" tint="0.39988402966399123"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,192 +489,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -889,262 +580,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1156,42 +608,126 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,134 +737,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1586,250 +1007,250 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12380952380952" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.37142857142857" customWidth="1"/>
-    <col min="2" max="2" width="11.1238095238095" customWidth="1"/>
-    <col min="3" max="3" width="42.247619047619" style="27" customWidth="1"/>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="42.25" style="23" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16" style="27" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="23" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="13.8761904761905" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.752380952381"/>
-    <col min="10" max="10" width="14.752380952381" style="6"/>
-    <col min="11" max="11" width="13.5714285714286"/>
+    <col min="7" max="7" width="13.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.75"/>
+    <col min="10" max="10" width="14.75" style="6"/>
+    <col min="11" max="11" width="13.625"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" customHeight="1" spans="1:8">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:10" ht="36" customHeight="1">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="28"/>
-    </row>
-    <row r="3" ht="21.95" customHeight="1" spans="1:8">
-      <c r="A3" s="31" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="3" spans="1:10" ht="21.95" customHeight="1">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" ht="15.75" spans="1:10">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="31" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="17">
+    <row r="5" spans="1:10">
+      <c r="A5" s="16">
         <v>1</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="26">
         <v>43112</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="14">
+      <c r="E5" s="27"/>
+      <c r="F5" s="13">
         <v>25000000</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <f>F5-G5</f>
         <v>25000000</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="17">
+    <row r="6" spans="1:10">
+      <c r="A6" s="16">
         <f t="shared" ref="A6:A24" si="0">A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="26">
         <v>43112</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="14">
+      <c r="E6" s="27"/>
+      <c r="F6" s="13">
         <v>1291000</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <f t="shared" ref="H6:H18" si="1">H5+F6-G6</f>
         <v>26291000</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="17">
+    <row r="7" spans="1:10">
+      <c r="A7" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="26">
         <v>43112</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14">
+      <c r="E7" s="27"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13">
         <v>1291000</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <f t="shared" si="1"/>
         <v>25000000</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="17">
+    <row r="8" spans="1:10">
+      <c r="A8" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="26">
         <v>43113</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14">
+      <c r="E8" s="27"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13">
         <v>5000000</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <f t="shared" si="1"/>
         <v>20000000</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="17">
+    <row r="9" spans="1:10">
+      <c r="A9" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="26">
         <v>43113</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14">
+      <c r="E9" s="27"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13">
         <v>6500</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <f t="shared" si="1"/>
         <v>19993500</v>
       </c>
     </row>
-    <row r="10" ht="30" spans="1:8">
-      <c r="A10" s="17">
+    <row r="10" spans="1:10" ht="30">
+      <c r="A10" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="26">
         <v>43114</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14">
+      <c r="E10" s="27"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13">
         <v>1000000</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <f t="shared" si="1"/>
         <v>18993500</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="1:10">
-      <c r="A11" s="17">
+    <row r="11" spans="1:10" ht="30">
+      <c r="A11" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="26">
         <v>43115</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14">
+      <c r="F11" s="13"/>
+      <c r="G11" s="13">
         <v>25000000</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <f t="shared" si="1"/>
         <v>-6006500</v>
       </c>
@@ -1837,150 +1258,150 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="17">
+    <row r="12" spans="1:10">
+      <c r="A12" s="16">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" s="38">
+      <c r="B12" s="26">
         <v>43115</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>5000000</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13">
         <f t="shared" si="1"/>
         <v>-1006500</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="17">
+    <row r="13" spans="1:10">
+      <c r="A13" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="26">
         <v>43115</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="14">
+      <c r="E13" s="27"/>
+      <c r="F13" s="13">
         <v>25000000</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13">
         <f t="shared" si="1"/>
         <v>23993500</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="17">
+    <row r="14" spans="1:10">
+      <c r="A14" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B14" s="38">
+      <c r="B14" s="26">
         <v>43115</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="14">
+      <c r="E14" s="27"/>
+      <c r="F14" s="13">
         <v>25000000</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13">
         <f t="shared" si="1"/>
         <v>48993500</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="17">
+    <row r="15" spans="1:10">
+      <c r="A15" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B15" s="38">
+      <c r="B15" s="26">
         <v>43115</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="14">
+      <c r="E15" s="27"/>
+      <c r="F15" s="13">
         <v>25000000</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13">
         <f t="shared" si="1"/>
         <v>73993500</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="17">
+    <row r="16" spans="1:10">
+      <c r="A16" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="26">
         <v>43115</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14">
+      <c r="E16" s="27"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13">
         <v>1500000</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <f t="shared" si="1"/>
         <v>72493500</v>
       </c>
     </row>
-    <row r="17" ht="30" spans="1:10">
-      <c r="A17" s="17">
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="26">
         <v>43116</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14">
+      <c r="F17" s="13"/>
+      <c r="G17" s="13">
         <v>5000000</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="13">
         <f t="shared" si="1"/>
         <v>67493500</v>
       </c>
@@ -1988,484 +1409,484 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="17">
+    <row r="18" spans="1:10">
+      <c r="A18" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B18" s="38">
+      <c r="B18" s="26">
         <v>43116</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14">
+      <c r="E18" s="27"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13">
         <v>500000</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <f t="shared" si="1"/>
         <v>66993500</v>
       </c>
     </row>
-    <row r="19" ht="30" spans="1:8">
-      <c r="A19" s="17">
+    <row r="19" spans="1:10">
+      <c r="A19" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="26">
         <v>43116</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="D19" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14">
+      <c r="E19" s="27"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13">
         <v>5000000</v>
       </c>
-      <c r="H19" s="14">
-        <f t="shared" ref="H19:H61" si="2">H18+F19-G19</f>
+      <c r="H19" s="13">
+        <f t="shared" ref="H19:H66" si="2">H18+F19-G19</f>
         <v>61993500</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="17">
+    <row r="20" spans="1:10">
+      <c r="A20" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B20" s="38">
+      <c r="B20" s="26">
         <v>43116</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14">
+      <c r="E20" s="27"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13">
         <v>6500</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <f t="shared" si="2"/>
         <v>61987000</v>
       </c>
     </row>
-    <row r="21" ht="30" spans="1:8">
-      <c r="A21" s="17">
+    <row r="21" spans="1:10" ht="30">
+      <c r="A21" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B21" s="38">
+      <c r="B21" s="26">
         <v>43116</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14">
+      <c r="E21" s="27"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13">
         <v>20000000</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="13">
         <f t="shared" si="2"/>
         <v>41987000</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="17">
+    <row r="22" spans="1:10">
+      <c r="A22" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B22" s="38">
+      <c r="B22" s="26">
         <v>43116</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="14">
+      <c r="E22" s="27"/>
+      <c r="F22" s="13">
         <v>25000000</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14">
+      <c r="G22" s="13"/>
+      <c r="H22" s="13">
         <f t="shared" si="2"/>
         <v>66987000</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="17">
+    <row r="23" spans="1:10">
+      <c r="A23" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="26">
         <v>43116</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="14">
+      <c r="E23" s="27"/>
+      <c r="F23" s="13">
         <v>25000000</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13">
         <f t="shared" si="2"/>
         <v>91987000</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="17">
+    <row r="24" spans="1:10">
+      <c r="A24" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B24" s="26">
         <v>43116</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14">
+      <c r="E24" s="27"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13">
         <v>400000</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="13">
         <f t="shared" si="2"/>
         <v>91587000</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="17">
-        <f t="shared" ref="A25:A61" si="3">A24+1</f>
+    <row r="25" spans="1:10">
+      <c r="A25" s="16">
+        <f t="shared" ref="A25:A66" si="3">A24+1</f>
         <v>21</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="26">
         <v>43116</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="13">
         <v>5000000</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14">
+      <c r="G25" s="13"/>
+      <c r="H25" s="13">
         <f t="shared" si="2"/>
         <v>96587000</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="17">
+    <row r="26" spans="1:10">
+      <c r="A26" s="16">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B26" s="38">
+      <c r="B26" s="26">
         <v>43117</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="13">
         <v>620000</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14">
+      <c r="G26" s="13"/>
+      <c r="H26" s="13">
         <f t="shared" si="2"/>
         <v>97207000</v>
       </c>
     </row>
-    <row r="27" ht="30" spans="1:8">
-      <c r="A27" s="17">
+    <row r="27" spans="1:10" ht="30">
+      <c r="A27" s="16">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B27" s="26">
         <v>43117</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14">
+      <c r="E27" s="27"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13">
         <v>15000000</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="13">
         <f t="shared" si="2"/>
         <v>82207000</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="17">
+    <row r="28" spans="1:10">
+      <c r="A28" s="16">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B28" s="38">
+      <c r="B28" s="26">
         <v>43117</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="14">
+      <c r="E28" s="27"/>
+      <c r="F28" s="13">
         <v>2000000</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13">
         <f t="shared" si="2"/>
         <v>84207000</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="17">
+    <row r="29" spans="1:10">
+      <c r="A29" s="16">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="26">
         <v>43117</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14">
+      <c r="E29" s="27"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13">
         <v>2000000</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="13">
         <f t="shared" si="2"/>
         <v>82207000</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="17">
+    <row r="30" spans="1:10">
+      <c r="A30" s="16">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="26">
         <v>43117</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14">
+      <c r="E30" s="27"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13">
         <v>4000000</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="13">
         <f t="shared" si="2"/>
         <v>78207000</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="17">
+    <row r="31" spans="1:10">
+      <c r="A31" s="16">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B31" s="38">
+      <c r="B31" s="26">
         <v>43117</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14">
+      <c r="E31" s="27"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13">
         <v>500000</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="13">
         <f t="shared" si="2"/>
         <v>77707000</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="17">
+    <row r="32" spans="1:10">
+      <c r="A32" s="16">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B32" s="38">
+      <c r="B32" s="26">
         <v>43117</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14">
+      <c r="E32" s="27"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13">
         <v>5000000</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="13">
         <f t="shared" si="2"/>
         <v>72707000</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="17">
+    <row r="33" spans="1:10">
+      <c r="A33" s="16">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="26">
         <v>43117</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14">
+      <c r="E33" s="27"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13">
         <v>6500</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="13">
         <f t="shared" si="2"/>
         <v>72700500</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="17">
+    <row r="34" spans="1:10">
+      <c r="A34" s="16">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B34" s="26">
         <v>43117</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C34" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="39" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="13">
         <v>1000000</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14">
+      <c r="G34" s="13"/>
+      <c r="H34" s="13">
         <f t="shared" si="2"/>
         <v>73700500</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="17">
+    <row r="35" spans="1:10">
+      <c r="A35" s="16">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B35" s="26">
         <v>43117</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="39" t="s">
+      <c r="D35" s="16"/>
+      <c r="E35" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="13">
         <v>1000000</v>
       </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14">
+      <c r="G35" s="13"/>
+      <c r="H35" s="13">
         <f t="shared" si="2"/>
         <v>74700500</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="17">
+    <row r="36" spans="1:10">
+      <c r="A36" s="16">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B36" s="38">
+      <c r="B36" s="26">
         <v>43117</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="42">
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="30">
         <v>100000</v>
       </c>
-      <c r="G36" s="42"/>
-      <c r="H36" s="14">
+      <c r="G36" s="30"/>
+      <c r="H36" s="13">
         <f t="shared" si="2"/>
         <v>74800500</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="17">
+      <c r="A37" s="16">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B37" s="26">
         <v>43118</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14">
+      <c r="E37" s="27"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13">
         <v>15000000</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H37" s="13">
         <f t="shared" si="2"/>
         <v>59800500</v>
       </c>
@@ -2473,142 +1894,142 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="38" ht="30" spans="1:8">
-      <c r="A38" s="17">
+    <row r="38" spans="1:10" ht="30">
+      <c r="A38" s="16">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="B38" s="38">
+      <c r="B38" s="26">
         <v>43118</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E38" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14">
+      <c r="F38" s="13"/>
+      <c r="G38" s="13">
         <v>5000000</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="13">
         <f t="shared" si="2"/>
         <v>54800500</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="17">
+    <row r="39" spans="1:10">
+      <c r="A39" s="16">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B39" s="38">
+      <c r="B39" s="26">
         <v>43119</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="14">
+      <c r="D39" s="16"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="13">
         <v>25000000</v>
       </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14">
+      <c r="G39" s="13"/>
+      <c r="H39" s="13">
         <f t="shared" si="2"/>
         <v>79800500</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="17">
+    <row r="40" spans="1:10">
+      <c r="A40" s="16">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="B40" s="38">
+      <c r="B40" s="26">
         <v>43119</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="14">
+      <c r="D40" s="16"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="13">
         <v>25000000</v>
       </c>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14">
+      <c r="G40" s="13"/>
+      <c r="H40" s="13">
         <f t="shared" si="2"/>
         <v>104800500</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="17">
+    <row r="41" spans="1:10">
+      <c r="A41" s="16">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="B41" s="38">
+      <c r="B41" s="26">
         <v>43119</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="39" t="s">
+      <c r="D41" s="16"/>
+      <c r="E41" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="13">
         <v>1000000</v>
       </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14">
+      <c r="G41" s="13"/>
+      <c r="H41" s="13">
         <f t="shared" si="2"/>
         <v>105800500</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="17">
+    <row r="42" spans="1:10">
+      <c r="A42" s="16">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="B42" s="38">
+      <c r="B42" s="26">
         <v>43120</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="39" t="s">
+      <c r="D42" s="16"/>
+      <c r="E42" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="14">
+      <c r="F42" s="13">
         <v>200000</v>
       </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14">
+      <c r="G42" s="13"/>
+      <c r="H42" s="13">
         <f t="shared" si="2"/>
         <v>106000500</v>
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="17">
+      <c r="A43" s="16">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="B43" s="38">
+      <c r="B43" s="26">
         <v>43120</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14">
+      <c r="D43" s="16"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13">
         <v>5000000</v>
       </c>
-      <c r="H43" s="14">
+      <c r="H43" s="13">
         <f t="shared" si="2"/>
         <v>101000500</v>
       </c>
@@ -2617,337 +2038,337 @@
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="17">
+      <c r="A44" s="16">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="B44" s="38">
+      <c r="B44" s="26">
         <v>43120</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="39" t="s">
+      <c r="D44" s="16"/>
+      <c r="E44" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F44" s="14">
+      <c r="F44" s="13">
         <v>3405000</v>
       </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14">
+      <c r="G44" s="13"/>
+      <c r="H44" s="13">
         <f t="shared" si="2"/>
         <v>104405500</v>
       </c>
       <c r="J44"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="17">
+      <c r="A45" s="16">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="B45" s="38">
+      <c r="B45" s="26">
         <v>43120</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C45" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="39" t="s">
+      <c r="D45" s="16"/>
+      <c r="E45" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="13">
         <v>500000</v>
       </c>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14">
+      <c r="G45" s="13"/>
+      <c r="H45" s="13">
         <f t="shared" si="2"/>
         <v>104905500</v>
       </c>
       <c r="J45"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="17">
+      <c r="A46" s="16">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="B46" s="38">
+      <c r="B46" s="26">
         <v>43120</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="14">
+      <c r="D46" s="16"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="13">
         <v>1000000</v>
       </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14">
+      <c r="G46" s="13"/>
+      <c r="H46" s="13">
         <f t="shared" si="2"/>
         <v>105905500</v>
       </c>
       <c r="J46"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="17">
+      <c r="A47" s="16">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="B47" s="38">
+      <c r="B47" s="26">
         <v>43120</v>
       </c>
-      <c r="C47" s="39" t="s">
+      <c r="C47" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14">
+      <c r="D47" s="16"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13">
         <v>1000000</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="13">
         <f t="shared" si="2"/>
         <v>104905500</v>
       </c>
       <c r="J47"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="17">
+      <c r="A48" s="16">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="B48" s="38">
+      <c r="B48" s="26">
         <v>43120</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="14">
+      <c r="D48" s="16"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="13">
         <v>300000</v>
       </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14">
+      <c r="G48" s="13"/>
+      <c r="H48" s="13">
         <f t="shared" si="2"/>
         <v>105205500</v>
       </c>
       <c r="J48"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="17">
+      <c r="A49" s="16">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="B49" s="38">
+      <c r="B49" s="26">
         <v>43120</v>
       </c>
-      <c r="C49" s="39" t="s">
+      <c r="C49" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="14">
+      <c r="D49" s="16"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="13">
         <v>200000</v>
       </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14">
+      <c r="G49" s="13"/>
+      <c r="H49" s="13">
         <f t="shared" si="2"/>
         <v>105405500</v>
       </c>
       <c r="J49"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="17">
+      <c r="A50" s="16">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="B50" s="38">
+      <c r="B50" s="26">
         <v>43120</v>
       </c>
-      <c r="C50" s="39" t="s">
+      <c r="C50" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="14">
+      <c r="D50" s="16"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="13">
         <v>200000</v>
       </c>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14">
+      <c r="G50" s="13"/>
+      <c r="H50" s="13">
         <f t="shared" si="2"/>
         <v>105605500</v>
       </c>
       <c r="J50"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="17">
+      <c r="A51" s="16">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="B51" s="38">
+      <c r="B51" s="26">
         <v>43120</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C51" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="42">
+      <c r="D51" s="16"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="30">
         <v>5000000</v>
       </c>
-      <c r="H51" s="14">
+      <c r="H51" s="13">
         <f t="shared" si="2"/>
         <v>100605500</v>
       </c>
       <c r="J51"/>
     </row>
-    <row r="52" ht="45" spans="1:10">
-      <c r="A52" s="17">
+    <row r="52" spans="1:10" ht="45">
+      <c r="A52" s="16">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="B52" s="38">
+      <c r="B52" s="26">
         <v>43120</v>
       </c>
-      <c r="C52" s="39" t="s">
+      <c r="C52" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E52" s="39" t="s">
+      <c r="E52" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14">
+      <c r="F52" s="13"/>
+      <c r="G52" s="13">
         <v>1000000</v>
       </c>
-      <c r="H52" s="14">
+      <c r="H52" s="13">
         <f t="shared" si="2"/>
         <v>99605500</v>
       </c>
       <c r="J52"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="17">
+      <c r="A53" s="16">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="B53" s="38">
+      <c r="B53" s="26">
         <v>43120</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="39"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14">
+      <c r="E53" s="27"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13">
         <v>20000000</v>
       </c>
-      <c r="H53" s="14">
+      <c r="H53" s="13">
         <f t="shared" si="2"/>
         <v>79605500</v>
       </c>
       <c r="J53"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="17">
+      <c r="A54" s="16">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="B54" s="38">
+      <c r="B54" s="26">
         <v>43121</v>
       </c>
-      <c r="C54" s="39" t="s">
+      <c r="C54" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="39"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14">
+      <c r="E54" s="27"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13">
         <v>4520000</v>
       </c>
-      <c r="H54" s="14">
+      <c r="H54" s="13">
         <f t="shared" si="2"/>
         <v>75085500</v>
       </c>
       <c r="J54"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="17">
+      <c r="A55" s="16">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="B55" s="38">
+      <c r="B55" s="26">
         <v>43121</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="C55" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14">
+      <c r="E55" s="27"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13">
         <v>1800000</v>
       </c>
-      <c r="H55" s="14">
+      <c r="H55" s="13">
         <f t="shared" si="2"/>
         <v>73285500</v>
       </c>
       <c r="J55"/>
     </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="17">
+    <row r="56" spans="1:10">
+      <c r="A56" s="16">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="B56" s="38">
+      <c r="B56" s="26">
         <v>43121</v>
       </c>
-      <c r="C56" s="39" t="s">
+      <c r="C56" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="14">
+      <c r="D56" s="16"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="13">
         <v>620000</v>
       </c>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14">
+      <c r="G56" s="13"/>
+      <c r="H56" s="13">
         <f t="shared" si="2"/>
         <v>73905500</v>
       </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="17">
+      <c r="A57" s="16">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
-      <c r="B57" s="38">
+      <c r="B57" s="26">
         <v>43121</v>
       </c>
-      <c r="C57" s="39" t="s">
+      <c r="C57" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="39"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14">
+      <c r="E57" s="27"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13">
         <v>3000000</v>
       </c>
-      <c r="H57" s="14">
+      <c r="H57" s="13">
         <f t="shared" si="2"/>
         <v>70905500</v>
       </c>
@@ -2955,143 +2376,239 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="17">
+    <row r="58" spans="1:10">
+      <c r="A58" s="16">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="B58" s="38">
+      <c r="B58" s="26">
         <v>43121</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="C58" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D58" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="39"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14">
+      <c r="E58" s="27"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13">
         <v>20000000</v>
       </c>
-      <c r="H58" s="14">
+      <c r="H58" s="13">
         <f t="shared" si="2"/>
         <v>50905500</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="17">
+    <row r="59" spans="1:10">
+      <c r="A59" s="16">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
-      <c r="B59" s="38">
+      <c r="B59" s="26">
         <v>43121</v>
       </c>
-      <c r="C59" s="39" t="s">
+      <c r="C59" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E59" s="39"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14">
+      <c r="E59" s="27"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13">
         <v>500000</v>
       </c>
-      <c r="H59" s="14">
+      <c r="H59" s="13">
         <f t="shared" si="2"/>
         <v>50405500</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="17">
+    <row r="60" spans="1:10">
+      <c r="A60" s="16">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="B60" s="38">
+      <c r="B60" s="26">
         <v>43121</v>
       </c>
-      <c r="C60" s="39" t="s">
+      <c r="C60" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="39"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14">
+      <c r="E60" s="27"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13">
         <v>5000000</v>
       </c>
-      <c r="H60" s="14">
+      <c r="H60" s="13">
         <f t="shared" si="2"/>
         <v>45405500</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="17">
+    <row r="61" spans="1:10">
+      <c r="A61" s="16">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
-      <c r="B61" s="38">
+      <c r="B61" s="26">
         <v>43121</v>
       </c>
-      <c r="C61" s="39" t="s">
+      <c r="C61" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="17"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="14">
+      <c r="D61" s="16"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="13">
         <v>25000000</v>
       </c>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14">
+      <c r="G61" s="13"/>
+      <c r="H61" s="13">
         <f t="shared" si="2"/>
         <v>70405500</v>
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="16">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="B62" s="26">
+        <v>43122</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" s="27"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13">
+        <v>500000</v>
+      </c>
+      <c r="H62" s="13">
+        <f t="shared" si="2"/>
+        <v>69905500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="16">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="B63" s="26">
+        <v>43122</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E63" s="27"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13">
+        <v>6500</v>
+      </c>
+      <c r="H63" s="13">
+        <f t="shared" si="2"/>
+        <v>69899000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="16">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="B64" s="26"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13">
+        <f t="shared" si="2"/>
+        <v>69899000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="16">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="B65" s="26"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13">
+        <f t="shared" si="2"/>
+        <v>69899000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="16">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="B66" s="26"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13">
+        <f t="shared" si="2"/>
+        <v>69899000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="13">
-        <f>SUM(F5:F61)</f>
+      <c r="B67" s="38"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="12">
+        <f>SUM(F5:F66)</f>
         <v>248436000</v>
       </c>
-      <c r="G62" s="13">
-        <f>SUM(G5:G61)</f>
-        <v>178030500</v>
-      </c>
-      <c r="H62" s="13" t="b">
-        <f>H61=(F62-G62)</f>
+      <c r="G67" s="12">
+        <f>SUM(G5:G66)</f>
+        <v>178537000</v>
+      </c>
+      <c r="H67" s="12" t="b">
+        <f>(F67-G67)=H66</f>
         <v>1</v>
       </c>
-      <c r="J62" s="6">
+      <c r="J67" s="6">
         <f>SUM(J5:J61)</f>
         <v>38000000</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
+    <row r="69" spans="1:10">
+      <c r="A69" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65">
+    <row r="70" spans="1:10">
+      <c r="A70">
         <v>1</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66">
+    <row r="71" spans="1:10">
+      <c r="A71">
         <v>2</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B71" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3099,85 +2616,83 @@
   <mergeCells count="8">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A67:C67"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12380952380952" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="32.247619047619" customWidth="1"/>
-    <col min="3" max="3" width="15.752380952381"/>
-    <col min="4" max="4" width="24.1238095238095" customWidth="1"/>
-    <col min="6" max="6" width="56.8761904761905" customWidth="1"/>
-    <col min="7" max="7" width="16.752380952381" customWidth="1"/>
+    <col min="2" max="2" width="32.25" customWidth="1"/>
+    <col min="3" max="3" width="15.75"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="6" max="6" width="56.875" customWidth="1"/>
+    <col min="7" max="7" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="10" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="F5" s="15" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <f>50000*4*385</f>
         <v>77000000</v>
       </c>
@@ -3186,21 +2701,21 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>1</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <f>G9</f>
         <v>106200000</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="F6" s="17" t="s">
+      <c r="D6" s="13"/>
+      <c r="F6" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f>4*4*250000</f>
         <v>4000000</v>
       </c>
@@ -3209,20 +2724,20 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>2</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>6000000</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="F7" s="17" t="s">
+      <c r="D7" s="13"/>
+      <c r="F7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <f>6000000*4</f>
         <v>24000000</v>
       </c>
@@ -3230,442 +2745,442 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="17">
+    <row r="8" spans="1:9">
+      <c r="A8" s="16">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>1000000</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="F8" s="17" t="s">
+      <c r="D8" s="13"/>
+      <c r="F8" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <f>300000*4</f>
         <v>1200000</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="17"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="16"/>
+      <c r="B9" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <f>SUM(C6:C8)</f>
         <v>113200000</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>125000000</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <f>SUM(G5:G8)</f>
         <v>106200000</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="17"/>
-      <c r="B11" s="12" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="16"/>
       <c r="F11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="17">
+    <row r="12" spans="1:9">
+      <c r="A12" s="16">
         <v>1</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>3000000</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>3000000</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="17">
+    <row r="13" spans="1:9">
+      <c r="A13" s="16">
         <v>2</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>68000000</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>5000000</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="18" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="17">
+    <row r="14" spans="1:9">
+      <c r="A14" s="16">
         <v>3</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <f>13700000+25000000</f>
         <v>38700000</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>40000000</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="17">
+    <row r="15" spans="1:9">
+      <c r="A15" s="16">
         <v>4</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="13">
         <v>113415000</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>113500000</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="18" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="17">
+    <row r="16" spans="1:9">
+      <c r="A16" s="16">
         <v>5</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <v>1000000</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>3000000</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="17">
+    <row r="17" spans="1:7">
+      <c r="A17" s="16">
         <v>6</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>3000000</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="13">
         <v>3000000</v>
       </c>
       <c r="F17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="17">
+    <row r="18" spans="1:7">
+      <c r="A18" s="16">
         <v>7</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>500000</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>5000000</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="17">
+    <row r="19" spans="1:7">
+      <c r="A19" s="16">
         <v>8</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <v>3000000</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="13">
         <v>5000000</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="17">
+    <row r="20" spans="1:7">
+      <c r="A20" s="16">
         <v>9</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="13">
         <v>5000000</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="13">
         <v>2000000</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="17">
+    <row r="21" spans="1:7">
+      <c r="A21" s="16">
         <v>10</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13">
         <v>50000000</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="17">
+    <row r="22" spans="1:7">
+      <c r="A22" s="16">
         <v>11</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>2000000</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <v>3000000</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="17"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="12">
         <f>SUM(C12:C22)</f>
         <v>237615000</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="12">
         <f>SUM(D12:D22)</f>
         <v>232500000</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="21">
         <f>250000*300</f>
         <v>75000000</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="17"/>
+    <row r="24" spans="1:7">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="17"/>
-      <c r="B25" s="12" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="22">
         <f>C9+C23</f>
         <v>350815000</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="22">
         <f>D9+D23</f>
         <v>357500000</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="21">
         <f>C25-G23</f>
         <v>275815000</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="17"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="17"/>
-    </row>
-    <row r="30" spans="3:3">
-      <c r="C30" s="25"/>
-    </row>
-    <row r="31" spans="3:3">
-      <c r="C31" s="25"/>
-    </row>
-    <row r="32" spans="3:3">
-      <c r="C32" s="25"/>
+    <row r="26" spans="1:7">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="C32" s="21"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="25"/>
+      <c r="C33" s="21"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="25"/>
+      <c r="C34" s="21"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="25"/>
+      <c r="C35" s="21"/>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="25"/>
+      <c r="C36" s="21"/>
     </row>
     <row r="37" spans="3:3">
-      <c r="C37" s="25"/>
+      <c r="C37" s="21"/>
     </row>
     <row r="38" spans="3:3">
-      <c r="C38" s="25"/>
+      <c r="C38" s="21"/>
     </row>
     <row r="39" spans="3:3">
-      <c r="C39" s="25"/>
+      <c r="C39" s="21"/>
     </row>
     <row r="40" spans="3:3">
-      <c r="C40" s="25"/>
+      <c r="C40" s="21"/>
     </row>
     <row r="41" spans="3:3">
-      <c r="C41" s="25"/>
+      <c r="C41" s="21"/>
     </row>
     <row r="42" spans="3:3">
-      <c r="C42" s="25"/>
+      <c r="C42" s="21"/>
     </row>
     <row r="43" spans="3:3">
-      <c r="C43" s="25"/>
+      <c r="C43" s="21"/>
     </row>
     <row r="44" spans="3:3">
-      <c r="C44" s="25"/>
+      <c r="C44" s="21"/>
     </row>
     <row r="45" spans="3:3">
-      <c r="C45" s="25"/>
+      <c r="C45" s="21"/>
     </row>
     <row r="46" spans="3:3">
-      <c r="C46" s="25"/>
+      <c r="C46" s="21"/>
     </row>
     <row r="47" spans="3:3">
-      <c r="C47" s="25"/>
+      <c r="C47" s="21"/>
     </row>
     <row r="48" spans="3:3">
-      <c r="C48" s="25"/>
+      <c r="C48" s="21"/>
     </row>
     <row r="49" spans="3:3">
-      <c r="C49" s="25"/>
+      <c r="C49" s="21"/>
     </row>
     <row r="50" spans="3:3">
-      <c r="C50" s="25"/>
+      <c r="C50" s="21"/>
     </row>
     <row r="51" spans="3:3">
-      <c r="C51" s="25"/>
+      <c r="C51" s="21"/>
     </row>
     <row r="52" spans="3:3">
-      <c r="C52" s="25"/>
+      <c r="C52" s="21"/>
     </row>
     <row r="53" spans="3:3">
-      <c r="C53" s="25"/>
+      <c r="C53" s="21"/>
     </row>
     <row r="54" spans="3:3">
-      <c r="C54" s="25"/>
+      <c r="C54" s="21"/>
     </row>
     <row r="55" spans="3:3">
-      <c r="C55" s="25"/>
+      <c r="C55" s="21"/>
     </row>
     <row r="56" spans="3:3">
-      <c r="C56" s="25"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="3:3">
-      <c r="C57" s="25"/>
+      <c r="C57" s="21"/>
     </row>
     <row r="58" spans="3:3">
-      <c r="C58" s="25"/>
+      <c r="C58" s="21"/>
     </row>
     <row r="59" spans="3:3">
-      <c r="C59" s="25"/>
+      <c r="C59" s="21"/>
     </row>
     <row r="60" spans="3:3">
-      <c r="C60" s="25"/>
+      <c r="C60" s="21"/>
     </row>
     <row r="61" spans="3:3">
-      <c r="C61" s="25"/>
+      <c r="C61" s="21"/>
     </row>
     <row r="62" spans="3:3">
-      <c r="C62" s="25"/>
+      <c r="C62" s="21"/>
     </row>
     <row r="63" spans="3:3">
-      <c r="C63" s="25"/>
+      <c r="C63" s="21"/>
     </row>
     <row r="64" spans="3:3">
-      <c r="C64" s="25"/>
+      <c r="C64" s="21"/>
     </row>
     <row r="65" spans="3:3">
-      <c r="C65" s="25"/>
+      <c r="C65" s="21"/>
     </row>
     <row r="66" spans="3:3">
-      <c r="C66" s="25"/>
+      <c r="C66" s="21"/>
     </row>
     <row r="67" spans="3:3">
-      <c r="C67" s="25"/>
+      <c r="C67" s="21"/>
     </row>
     <row r="68" spans="3:3">
-      <c r="C68" s="25"/>
+      <c r="C68" s="21"/>
     </row>
     <row r="69" spans="3:3">
-      <c r="C69" s="25"/>
+      <c r="C69" s="21"/>
     </row>
     <row r="70" spans="3:3">
-      <c r="C70" s="25"/>
+      <c r="C70" s="21"/>
     </row>
     <row r="71" spans="3:3">
-      <c r="C71" s="25"/>
+      <c r="C71" s="21"/>
     </row>
     <row r="72" spans="3:3">
-      <c r="C72" s="25"/>
+      <c r="C72" s="21"/>
     </row>
     <row r="73" spans="3:3">
-      <c r="C73" s="25"/>
+      <c r="C73" s="21"/>
     </row>
     <row r="74" spans="3:3">
-      <c r="C74" s="25"/>
+      <c r="C74" s="21"/>
     </row>
     <row r="75" spans="3:3">
-      <c r="C75" s="25"/>
+      <c r="C75" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3673,24 +3188,20 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A10:D10"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="15.7142857142857" style="7"/>
+    <col min="1" max="1" width="25.875" customWidth="1"/>
+    <col min="2" max="2" width="15.75" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -3755,26 +3266,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="63.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="10.5714285714286"/>
-    <col min="4" max="4" width="13.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="14.7142857142857" style="1"/>
+    <col min="1" max="1" width="63.75" customWidth="1"/>
+    <col min="2" max="2" width="10.625"/>
+    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="14.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3843,7 +3352,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
         <v>120</v>
       </c>
@@ -3851,7 +3360,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
         <v>121</v>
       </c>
@@ -3859,7 +3368,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
         <v>122</v>
       </c>
@@ -3867,7 +3376,7 @@
         <v>370000</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
         <v>123</v>
       </c>
@@ -3875,7 +3384,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
         <v>124</v>
       </c>
@@ -3883,7 +3392,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
         <v>125</v>
       </c>
@@ -3891,7 +3400,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
         <v>126</v>
       </c>
@@ -3899,7 +3408,7 @@
         <v>350000</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -3922,8 +3431,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Class dana daurah 23 Jan 2017
</commit_message>
<xml_diff>
--- a/Daurah Masyaikh Asrama Haji.xlsx
+++ b/Daurah Masyaikh Asrama Haji.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mutasi Kas" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="148">
   <si>
     <t>Mutasi Kas Daurah Masyaikh di Surakarta</t>
   </si>
@@ -457,6 +457,15 @@
   </si>
   <si>
     <t>Uang yang dipegang abu taqiyan Rp 44.000.000 dialokasikan untuk bayar asrama haji</t>
+  </si>
+  <si>
+    <t>Rincian Pembayaran</t>
+  </si>
+  <si>
+    <t>Cicilan I</t>
+  </si>
+  <si>
+    <t>Kurang Bayar</t>
   </si>
 </sst>
 </file>
@@ -468,7 +477,7 @@
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +520,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -641,7 +658,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -747,6 +764,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,13 +827,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1091,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
@@ -1110,45 +1148,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="21.95" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="38"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="46"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="26" t="s">
         <v>7</v>
       </c>
@@ -2816,11 +2854,11 @@
       </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="40" t="s">
+      <c r="A74" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="40"/>
-      <c r="C74" s="41"/>
+      <c r="B74" s="42"/>
+      <c r="C74" s="43"/>
       <c r="D74" s="19"/>
       <c r="E74" s="33"/>
       <c r="F74" s="11">
@@ -2852,7 +2890,7 @@
       <c r="B77" t="s">
         <v>144</v>
       </c>
-      <c r="F77" s="55"/>
+      <c r="F77" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2874,8 +2912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC75"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -2884,37 +2922,44 @@
     <col min="2" max="2" width="32.25" customWidth="1"/>
     <col min="3" max="3" width="15.75"/>
     <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="6" max="6" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="7" width="21.875" customWidth="1"/>
-    <col min="8" max="8" width="11.75"/>
+    <col min="8" max="8" width="13.75" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
     <col min="11" max="11" width="14.75"/>
     <col min="26" max="26" width="56.875" customWidth="1"/>
     <col min="27" max="27" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="F1" s="54" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="F1" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:29">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="9" t="s">
@@ -3144,10 +3189,10 @@
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="14"/>
@@ -3244,13 +3289,13 @@
       <c r="D14" s="12">
         <v>40000000</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
       <c r="K14" s="18">
         <f>SUM(K5:K13)</f>
         <v>83400000</v>
@@ -3289,6 +3334,9 @@
       <c r="D16" s="12">
         <v>3000000</v>
       </c>
+      <c r="F16" s="56" t="s">
+        <v>145</v>
+      </c>
       <c r="Z16" s="24" t="s">
         <v>113</v>
       </c>
@@ -3306,6 +3354,18 @@
       <c r="D17" s="12">
         <v>3000000</v>
       </c>
+      <c r="F17" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="62" t="s">
+        <v>6</v>
+      </c>
       <c r="Z17" t="s">
         <v>115</v>
       </c>
@@ -3323,6 +3383,19 @@
       <c r="D18" s="12">
         <v>5000000</v>
       </c>
+      <c r="F18" s="15">
+        <v>1</v>
+      </c>
+      <c r="G18" s="28">
+        <f>'Mutasi Kas'!B11</f>
+        <v>43115</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="16">
+        <v>20000000</v>
+      </c>
       <c r="Z18" s="22" t="s">
         <v>117</v>
       </c>
@@ -3340,6 +3413,19 @@
       <c r="D19" s="12">
         <v>5000000</v>
       </c>
+      <c r="F19" s="15">
+        <v>2</v>
+      </c>
+      <c r="G19" s="28">
+        <f>'Mutasi Kas'!B65</f>
+        <v>43122</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" s="16">
+        <v>30000000</v>
+      </c>
       <c r="Z19" s="22" t="s">
         <v>118</v>
       </c>
@@ -3357,6 +3443,10 @@
       <c r="D20" s="12">
         <v>2000000</v>
       </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="15">
@@ -3369,6 +3459,10 @@
       <c r="D21" s="12">
         <v>50000000</v>
       </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:27">
       <c r="A22" s="15">
@@ -3382,6 +3476,15 @@
       </c>
       <c r="D22" s="12">
         <v>3000000</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60">
+        <f>SUM(I18:I21)</f>
+        <v>50000000</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -3407,6 +3510,15 @@
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
       <c r="D24" s="15"/>
+      <c r="F24" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="63">
+        <f>K14-I22</f>
+        <v>33400000</v>
+      </c>
     </row>
     <row r="25" spans="1:27">
       <c r="A25" s="15"/>
@@ -3589,14 +3701,17 @@
       <c r="C75" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F24:H24"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="F1:K2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3604,7 +3719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -3622,7 +3737,7 @@
       <c r="B2" s="7">
         <v>45448633</v>
       </c>
-      <c r="D2" s="56">
+      <c r="D2" s="36">
         <f>B2+B3+B4</f>
         <v>2448633</v>
       </c>

</xml_diff>

<commit_message>
update dana keuangan darnas dan mahad
</commit_message>
<xml_diff>
--- a/Daurah Masyaikh Asrama Haji.xlsx
+++ b/Daurah Masyaikh Asrama Haji.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189">
   <si>
     <t>Mutasi Kas Daurah Masyaikh di Surakarta</t>
   </si>
@@ -246,6 +246,15 @@
     <t>Pembayaran sewa asrama haji</t>
   </si>
   <si>
+    <t>Penyerahan dana ke sie kebersihan melalui petugas dana</t>
+  </si>
+  <si>
+    <t>Aqua Ibrahim</t>
+  </si>
+  <si>
+    <t>Terima Dana dari Pak Sonhaji</t>
+  </si>
+  <si>
     <t>Pembelian pulsa syaikh</t>
   </si>
   <si>
@@ -255,6 +264,15 @@
     <t>Pembelian roti / snack</t>
   </si>
   <si>
+    <t>Transfer ke sie konsumsi</t>
+  </si>
+  <si>
+    <t>Biaya transportasi ke Asrama Haji</t>
+  </si>
+  <si>
+    <t>Pembelian Amplop</t>
+  </si>
+  <si>
     <t>Menerima dana cash dari bendahara pusat</t>
   </si>
   <si>
@@ -477,10 +495,10 @@
     <t>Uang sendiri</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Excel</t>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>Catatan</t>
   </si>
   <si>
     <t>Selisih</t>
@@ -538,9 +556,6 @@
   </si>
   <si>
     <t>Sisa</t>
-  </si>
-  <si>
-    <t>Real</t>
   </si>
   <si>
     <t>Quota</t>
@@ -581,8 +596,8 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -624,14 +639,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -645,16 +660,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -662,52 +670,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -722,9 +684,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,8 +716,30 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -760,8 +752,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -800,13 +815,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,25 +857,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -854,7 +887,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -866,31 +953,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -902,67 +971,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,32 +1092,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -1121,15 +1110,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1157,12 +1137,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1180,130 +1195,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1804,10 +1819,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12380952380952" defaultRowHeight="15"/>
@@ -3008,11 +3023,11 @@
       <c r="E51" s="55"/>
       <c r="F51" s="24"/>
       <c r="G51" s="23">
-        <v>5000000</v>
+        <v>5100000</v>
       </c>
       <c r="H51" s="23">
         <f t="shared" si="2"/>
-        <v>100605500</v>
+        <v>100505500</v>
       </c>
       <c r="J51"/>
     </row>
@@ -3039,7 +3054,7 @@
       </c>
       <c r="H52" s="23">
         <f t="shared" si="2"/>
-        <v>99605500</v>
+        <v>99505500</v>
       </c>
       <c r="J52"/>
     </row>
@@ -3064,7 +3079,7 @@
       </c>
       <c r="H53" s="23">
         <f t="shared" si="2"/>
-        <v>79605500</v>
+        <v>79505500</v>
       </c>
       <c r="J53"/>
     </row>
@@ -3089,7 +3104,7 @@
       </c>
       <c r="H54" s="23">
         <f t="shared" si="2"/>
-        <v>75085500</v>
+        <v>74985500</v>
       </c>
       <c r="J54"/>
     </row>
@@ -3114,7 +3129,7 @@
       </c>
       <c r="H55" s="23">
         <f t="shared" si="2"/>
-        <v>73285500</v>
+        <v>73185500</v>
       </c>
       <c r="J55"/>
     </row>
@@ -3137,7 +3152,7 @@
       <c r="G56" s="23"/>
       <c r="H56" s="23">
         <f t="shared" si="2"/>
-        <v>73905500</v>
+        <v>73805500</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3161,7 +3176,7 @@
       </c>
       <c r="H57" s="23">
         <f t="shared" si="2"/>
-        <v>70905500</v>
+        <v>70805500</v>
       </c>
       <c r="J57" s="13">
         <v>3000000</v>
@@ -3188,7 +3203,7 @@
       </c>
       <c r="H58" s="23">
         <f t="shared" si="2"/>
-        <v>50905500</v>
+        <v>50805500</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3212,7 +3227,7 @@
       </c>
       <c r="H59" s="23">
         <f t="shared" si="2"/>
-        <v>50405500</v>
+        <v>50305500</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3236,7 +3251,7 @@
       </c>
       <c r="H60" s="23">
         <f t="shared" si="2"/>
-        <v>45405500</v>
+        <v>45305500</v>
       </c>
       <c r="J60" s="13">
         <v>5000000</v>
@@ -3261,7 +3276,7 @@
       <c r="G61" s="23"/>
       <c r="H61" s="23">
         <f t="shared" si="2"/>
-        <v>70405500</v>
+        <v>70305500</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3285,7 +3300,7 @@
       </c>
       <c r="H62" s="23">
         <f t="shared" si="2"/>
-        <v>69905500</v>
+        <v>69805500</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3309,7 +3324,7 @@
       </c>
       <c r="H63" s="23">
         <f t="shared" si="2"/>
-        <v>69899000</v>
+        <v>69799000</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3333,7 +3348,7 @@
       </c>
       <c r="H64" s="23">
         <f t="shared" si="2"/>
-        <v>54899000</v>
+        <v>54799000</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3357,31 +3372,31 @@
       </c>
       <c r="H65" s="23">
         <f t="shared" si="2"/>
-        <v>24899000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>24799000</v>
+      </c>
+    </row>
+    <row r="66" ht="30" spans="1:8">
       <c r="A66" s="24">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="B66" s="31">
-        <v>43123</v>
-      </c>
-      <c r="C66" s="55" t="s">
+        <v>43122</v>
+      </c>
+      <c r="C66" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D66" s="24" t="s">
-        <v>30</v>
+      <c r="D66" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="E66" s="55"/>
       <c r="F66" s="23"/>
       <c r="G66" s="23">
-        <v>200000</v>
+        <v>500000</v>
       </c>
       <c r="H66" s="23">
         <f t="shared" si="2"/>
-        <v>24699000</v>
+        <v>24299000</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3390,26 +3405,23 @@
         <v>63</v>
       </c>
       <c r="B67" s="31">
-        <v>43123</v>
-      </c>
-      <c r="C67" s="55" t="s">
+        <v>43122</v>
+      </c>
+      <c r="C67" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="24" t="s">
-        <v>17</v>
-      </c>
+      <c r="D67" s="3"/>
       <c r="E67" s="55"/>
       <c r="F67" s="23"/>
       <c r="G67" s="23">
-        <f>19000+12000+4000</f>
-        <v>35000</v>
+        <v>8000</v>
       </c>
       <c r="H67" s="23">
         <f t="shared" si="2"/>
-        <v>24664000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>24291000</v>
+      </c>
+    </row>
+    <row r="68" ht="30" spans="1:8">
       <c r="A68" s="24">
         <f t="shared" si="3"/>
         <v>64</v>
@@ -3417,21 +3429,20 @@
       <c r="B68" s="31">
         <v>43123</v>
       </c>
-      <c r="C68" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" s="24" t="s">
-        <v>15</v>
+      <c r="C68" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="E68" s="55"/>
       <c r="F68" s="23"/>
       <c r="G68" s="23">
-        <f>40000+13000+14000+5000</f>
-        <v>72000</v>
+        <v>550000</v>
       </c>
       <c r="H68" s="23">
         <f t="shared" si="2"/>
-        <v>24592000</v>
+        <v>23741000</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3442,20 +3453,20 @@
       <c r="B69" s="31">
         <v>43123</v>
       </c>
-      <c r="C69" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="24" t="s">
+      <c r="C69" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E69" s="55"/>
       <c r="F69" s="23">
-        <v>25000000</v>
+        <v>1230000</v>
       </c>
       <c r="G69" s="23"/>
       <c r="H69" s="23">
         <f t="shared" si="2"/>
-        <v>49592000</v>
+        <v>24971000</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3466,20 +3477,20 @@
       <c r="B70" s="31">
         <v>43123</v>
       </c>
-      <c r="C70" s="56" t="s">
-        <v>73</v>
+      <c r="C70" s="55" t="s">
+        <v>78</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E70" s="55"/>
       <c r="F70" s="23"/>
       <c r="G70" s="23">
-        <v>2000000</v>
+        <v>200000</v>
       </c>
       <c r="H70" s="23">
-        <f t="shared" si="2"/>
-        <v>47592000</v>
+        <f>H67+F70-G70</f>
+        <v>24091000</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3488,22 +3499,23 @@
         <v>67</v>
       </c>
       <c r="B71" s="31">
-        <v>43124</v>
+        <v>43123</v>
       </c>
       <c r="C71" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E71" s="55"/>
-      <c r="F71" s="23">
-        <v>34860000</v>
-      </c>
-      <c r="G71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23">
+        <f>19000+12000+4000</f>
+        <v>35000</v>
+      </c>
       <c r="H71" s="23">
-        <f t="shared" si="2"/>
-        <v>82452000</v>
+        <f t="shared" ref="H71:H90" si="4">H70+F71-G71</f>
+        <v>24056000</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3512,22 +3524,23 @@
         <v>68</v>
       </c>
       <c r="B72" s="31">
-        <v>43124</v>
+        <v>43123</v>
       </c>
       <c r="C72" s="55" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E72" s="55"/>
       <c r="F72" s="23"/>
       <c r="G72" s="23">
-        <v>23800000</v>
+        <f>40000+13000+14000+5000</f>
+        <v>72000</v>
       </c>
       <c r="H72" s="23">
-        <f t="shared" si="2"/>
-        <v>58652000</v>
+        <f t="shared" si="4"/>
+        <v>23984000</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3536,22 +3549,22 @@
         <v>69</v>
       </c>
       <c r="B73" s="31">
-        <v>43124</v>
+        <v>43123</v>
       </c>
       <c r="C73" s="55" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="D73" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E73" s="55"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23">
-        <v>20000</v>
-      </c>
+      <c r="F73" s="23">
+        <v>25000000</v>
+      </c>
+      <c r="G73" s="23"/>
       <c r="H73" s="23">
-        <f t="shared" si="2"/>
-        <v>58632000</v>
+        <f t="shared" si="4"/>
+        <v>48984000</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3560,245 +3573,380 @@
         <v>70</v>
       </c>
       <c r="B74" s="31">
-        <v>43124</v>
-      </c>
-      <c r="C74" s="55" t="s">
+        <v>43123</v>
+      </c>
+      <c r="C74" s="56" t="s">
         <v>81</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E74" s="55"/>
       <c r="F74" s="23"/>
       <c r="G74" s="23">
-        <v>19000000</v>
+        <v>2000000</v>
       </c>
       <c r="H74" s="23">
-        <f t="shared" si="2"/>
-        <v>39632000</v>
+        <f t="shared" si="4"/>
+        <v>46984000</v>
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="24">
-        <f t="shared" si="3"/>
-        <v>71</v>
-      </c>
+      <c r="A75" s="24"/>
       <c r="B75" s="31">
-        <v>43124</v>
-      </c>
-      <c r="C75" s="55" t="s">
+        <v>43123</v>
+      </c>
+      <c r="C75" s="56" t="s">
         <v>82</v>
       </c>
       <c r="D75" s="24"/>
       <c r="E75" s="55"/>
       <c r="F75" s="23"/>
       <c r="G75" s="23">
-        <v>10600000</v>
+        <v>31000</v>
       </c>
       <c r="H75" s="23">
-        <f t="shared" si="2"/>
-        <v>29032000</v>
+        <f t="shared" si="4"/>
+        <v>46953000</v>
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="24">
-        <f t="shared" si="3"/>
-        <v>72</v>
-      </c>
+      <c r="A76" s="24"/>
       <c r="B76" s="31">
-        <v>43124</v>
-      </c>
-      <c r="C76" s="55" t="s">
+        <v>43123</v>
+      </c>
+      <c r="C76" s="56" t="s">
         <v>83</v>
       </c>
       <c r="D76" s="24"/>
       <c r="E76" s="55"/>
-      <c r="F76" s="23">
-        <v>4500000</v>
-      </c>
-      <c r="G76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23">
+        <f>17000*8</f>
+        <v>136000</v>
+      </c>
       <c r="H76" s="23">
-        <f t="shared" si="2"/>
-        <v>33532000</v>
+        <f t="shared" si="4"/>
+        <v>46817000</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="24">
-        <f t="shared" si="3"/>
-        <v>73</v>
-      </c>
-      <c r="B77" s="31"/>
-      <c r="C77" s="55"/>
-      <c r="D77" s="24"/>
+        <f>A74+1</f>
+        <v>71</v>
+      </c>
+      <c r="B77" s="31">
+        <v>43124</v>
+      </c>
+      <c r="C77" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="E77" s="55"/>
-      <c r="F77" s="23"/>
+      <c r="F77" s="23">
+        <v>34860000</v>
+      </c>
       <c r="G77" s="23"/>
       <c r="H77" s="23">
-        <f t="shared" si="2"/>
-        <v>33532000</v>
+        <f t="shared" si="4"/>
+        <v>81677000</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="24">
-        <f t="shared" si="3"/>
-        <v>74</v>
-      </c>
-      <c r="B78" s="31"/>
-      <c r="C78" s="55"/>
-      <c r="D78" s="24"/>
+        <f t="shared" ref="A78:A89" si="5">A77+1</f>
+        <v>72</v>
+      </c>
+      <c r="B78" s="31">
+        <v>43124</v>
+      </c>
+      <c r="C78" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="E78" s="55"/>
       <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
+      <c r="G78" s="23">
+        <v>23800000</v>
+      </c>
       <c r="H78" s="23">
-        <f t="shared" si="2"/>
-        <v>33532000</v>
+        <f t="shared" si="4"/>
+        <v>57877000</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="24">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="B79" s="31"/>
-      <c r="C79" s="55"/>
-      <c r="D79" s="24"/>
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="B79" s="31">
+        <v>43124</v>
+      </c>
+      <c r="C79" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="E79" s="55"/>
       <c r="F79" s="23"/>
-      <c r="G79" s="23"/>
+      <c r="G79" s="23">
+        <v>20000</v>
+      </c>
       <c r="H79" s="23">
-        <f t="shared" si="2"/>
-        <v>33532000</v>
+        <f t="shared" si="4"/>
+        <v>57857000</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="24">
-        <f t="shared" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="55"/>
-      <c r="D80" s="24"/>
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="B80" s="31">
+        <v>43124</v>
+      </c>
+      <c r="C80" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="E80" s="55"/>
       <c r="F80" s="23"/>
-      <c r="G80" s="23"/>
+      <c r="G80" s="23">
+        <v>19000000</v>
+      </c>
       <c r="H80" s="23">
-        <f t="shared" si="2"/>
-        <v>33532000</v>
+        <f t="shared" si="4"/>
+        <v>38857000</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="24">
-        <f t="shared" si="3"/>
-        <v>77</v>
-      </c>
-      <c r="B81" s="31"/>
-      <c r="C81" s="55"/>
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="B81" s="31">
+        <v>43124</v>
+      </c>
+      <c r="C81" s="55" t="s">
+        <v>88</v>
+      </c>
       <c r="D81" s="24"/>
       <c r="E81" s="55"/>
       <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
+      <c r="G81" s="23">
+        <v>10600000</v>
+      </c>
       <c r="H81" s="23">
-        <f t="shared" si="2"/>
-        <v>33532000</v>
+        <f t="shared" si="4"/>
+        <v>28257000</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="24">
-        <f t="shared" si="3"/>
-        <v>78</v>
-      </c>
-      <c r="B82" s="31"/>
-      <c r="C82" s="55"/>
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="B82" s="31">
+        <v>43124</v>
+      </c>
+      <c r="C82" s="55" t="s">
+        <v>89</v>
+      </c>
       <c r="D82" s="24"/>
       <c r="E82" s="55"/>
-      <c r="F82" s="23"/>
+      <c r="F82" s="23">
+        <v>5100000</v>
+      </c>
       <c r="G82" s="23"/>
       <c r="H82" s="23">
-        <f t="shared" si="2"/>
-        <v>33532000</v>
+        <f t="shared" si="4"/>
+        <v>33357000</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="24">
-        <f t="shared" si="3"/>
-        <v>79</v>
+        <f t="shared" si="5"/>
+        <v>77</v>
       </c>
       <c r="B83" s="31"/>
-      <c r="C83" s="55" t="s">
-        <v>84</v>
-      </c>
+      <c r="C83" s="55"/>
       <c r="D83" s="24"/>
       <c r="E83" s="55"/>
       <c r="F83" s="23"/>
-      <c r="G83" s="23">
-        <v>6000000</v>
-      </c>
+      <c r="G83" s="23"/>
       <c r="H83" s="23">
-        <f>H82+F83-G83</f>
-        <v>27532000</v>
+        <f t="shared" si="4"/>
+        <v>33357000</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="24">
-        <f>A73+1</f>
-        <v>70</v>
+        <f t="shared" si="5"/>
+        <v>78</v>
       </c>
       <c r="B84" s="31"/>
-      <c r="C84" s="55" t="s">
-        <v>85</v>
-      </c>
+      <c r="C84" s="55"/>
       <c r="D84" s="24"/>
       <c r="E84" s="55"/>
       <c r="F84" s="23"/>
       <c r="G84" s="23"/>
       <c r="H84" s="23">
-        <f>H83+F84-G84</f>
-        <v>27532000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B85" s="1"/>
-      <c r="C85" s="58"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="58"/>
-      <c r="F85" s="22">
-        <f>SUM(F5:F84)</f>
-        <v>312796000</v>
-      </c>
-      <c r="G85" s="22">
-        <f>SUM(G5:G84)</f>
-        <v>285264000</v>
-      </c>
-      <c r="H85" s="22" t="b">
-        <f>(F85-G85)=H84</f>
-        <v>1</v>
-      </c>
-      <c r="J85" s="13">
+        <f t="shared" si="4"/>
+        <v>33357000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="24">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="B85" s="31"/>
+      <c r="C85" s="55"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="55"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23">
+        <f t="shared" si="4"/>
+        <v>33357000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="24">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="B86" s="31"/>
+      <c r="C86" s="55"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23">
+        <f t="shared" si="4"/>
+        <v>33357000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="24">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+      <c r="B87" s="31"/>
+      <c r="C87" s="55"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="23">
+        <f t="shared" si="4"/>
+        <v>33357000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="24">
+        <f t="shared" si="5"/>
+        <v>82</v>
+      </c>
+      <c r="B88" s="31"/>
+      <c r="C88" s="55"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23">
+        <f t="shared" si="4"/>
+        <v>33357000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="24">
+        <f t="shared" si="5"/>
+        <v>83</v>
+      </c>
+      <c r="B89" s="31"/>
+      <c r="C89" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D89" s="24"/>
+      <c r="E89" s="55"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23">
+        <v>6000000</v>
+      </c>
+      <c r="H89" s="23">
+        <f t="shared" si="4"/>
+        <v>27357000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="24">
+        <f>A79+1</f>
+        <v>74</v>
+      </c>
+      <c r="B90" s="31"/>
+      <c r="C90" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90" s="24"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23">
+        <f t="shared" si="4"/>
+        <v>27357000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="58"/>
+      <c r="F91" s="22">
+        <f>SUM(F5:F90)</f>
+        <v>314626000</v>
+      </c>
+      <c r="G91" s="22">
+        <f>SUM(G5:G90)</f>
+        <v>286589000</v>
+      </c>
+      <c r="H91" s="22" t="b">
+        <f>(F91-G91)=H90</f>
+        <v>0</v>
+      </c>
+      <c r="J91" s="13">
         <f>SUM(J5:J61)</f>
         <v>43000000</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88">
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94">
         <v>1</v>
       </c>
-      <c r="B88" t="s">
-        <v>88</v>
+      <c r="B94" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A91:C91"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -3839,18 +3987,18 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="20" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="20" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -3867,28 +4015,28 @@
         <v>6</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>6</v>
@@ -3897,7 +4045,7 @@
     <row r="5" spans="1:29">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="23"/>
@@ -3905,7 +4053,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="H5" s="25">
         <v>50000</v>
@@ -3921,14 +4069,14 @@
         <v>73650000</v>
       </c>
       <c r="Z5" s="39" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="AA5" s="40">
         <f>50000*4*385</f>
         <v>77000000</v>
       </c>
       <c r="AC5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -3936,7 +4084,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C6" s="23">
         <f>AA9</f>
@@ -3947,21 +4095,21 @@
         <v>2</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
       <c r="Z6" s="24" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="AA6" s="23">
         <f>4*4*250000</f>
         <v>4000000</v>
       </c>
       <c r="AC6" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -3969,7 +4117,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C7" s="23">
         <v>6000000</v>
@@ -3979,21 +4127,21 @@
         <v>3</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
       <c r="Z7" s="24" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="AA7" s="23">
         <f>6000000*4</f>
         <v>24000000</v>
       </c>
       <c r="AC7" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -4001,7 +4149,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C8" s="23">
         <v>1000000</v>
@@ -4011,7 +4159,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H8" s="25">
         <v>250000</v>
@@ -4027,7 +4175,7 @@
         <v>5250000</v>
       </c>
       <c r="Z8" s="24" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="AA8" s="23">
         <f>300000*4</f>
@@ -4037,7 +4185,7 @@
     <row r="9" spans="1:27">
       <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C9" s="22">
         <f>SUM(C6:C8)</f>
@@ -4050,7 +4198,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="H9" s="24">
         <v>25000</v>
@@ -4063,7 +4211,7 @@
       </c>
       <c r="K9" s="24"/>
       <c r="Z9" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="AA9" s="22">
         <f>SUM(AA5:AA8)</f>
@@ -4077,7 +4225,7 @@
       <c r="D10" s="28"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H10" s="25">
         <v>6000000</v>
@@ -4096,13 +4244,13 @@
     <row r="11" spans="1:26">
       <c r="A11" s="24"/>
       <c r="B11" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H11" s="25">
         <v>300000</v>
@@ -4118,7 +4266,7 @@
         <v>900000</v>
       </c>
       <c r="Z11" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -4126,7 +4274,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C12" s="23">
         <v>3000000</v>
@@ -4136,7 +4284,7 @@
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="24" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H12" s="25">
         <v>300</v>
@@ -4150,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="Z12" s="41" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -4176,7 +4324,7 @@
         <v>0</v>
       </c>
       <c r="Z13" s="41" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -4194,7 +4342,7 @@
         <v>40000000</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -4205,7 +4353,7 @@
         <v>97800000</v>
       </c>
       <c r="Z14" s="42" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -4222,7 +4370,7 @@
         <v>113500000</v>
       </c>
       <c r="Z15" s="41" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -4230,7 +4378,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C16" s="23">
         <v>1000000</v>
@@ -4239,7 +4387,7 @@
         <v>3000000</v>
       </c>
       <c r="Z16" s="43" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -4247,7 +4395,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C17" s="23">
         <v>3000000</v>
@@ -4259,26 +4407,26 @@
         <v>1</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H17" s="30" t="s">
         <v>2</v>
       </c>
       <c r="I17" s="30"/>
       <c r="J17" s="36" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="K17" s="30" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="Z17" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:26">
@@ -4286,7 +4434,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C18" s="23">
         <v>500000</v>
@@ -4307,7 +4455,7 @@
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
       <c r="Z18" s="41" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -4327,7 +4475,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
@@ -4336,7 +4484,7 @@
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
       <c r="Z19" s="41" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -4344,7 +4492,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C20" s="23">
         <v>5000000</v>
@@ -4354,7 +4502,7 @@
       </c>
       <c r="F20" s="24"/>
       <c r="G20" s="24" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="H20" s="31">
         <v>43122</v>
@@ -4382,7 +4530,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23">
@@ -4390,7 +4538,7 @@
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="H21" s="31">
         <v>43123</v>
@@ -4428,7 +4576,7 @@
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="24" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="H22" s="31">
         <v>43122</v>
@@ -4454,7 +4602,7 @@
     <row r="23" spans="1:27">
       <c r="A23" s="24"/>
       <c r="B23" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C23" s="22">
         <f>SUM(C12:C22)</f>
@@ -4466,7 +4614,7 @@
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="24" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="H23" s="31">
         <v>43122</v>
@@ -4501,7 +4649,7 @@
       <c r="D24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="24" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="H24" s="31">
         <v>43123</v>
@@ -4527,7 +4675,7 @@
     <row r="25" spans="1:27">
       <c r="A25" s="24"/>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C25" s="32">
         <f>C9+C23</f>
@@ -4539,7 +4687,7 @@
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H25" s="31">
         <v>43122</v>
@@ -4575,7 +4723,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
@@ -4591,7 +4739,7 @@
       <c r="D27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H27" s="31">
         <v>43122</v>
@@ -4620,7 +4768,7 @@
       <c r="D28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H28" s="31">
         <v>43122</v>
@@ -4649,7 +4797,7 @@
       <c r="D29" s="24"/>
       <c r="F29" s="33"/>
       <c r="G29" s="24" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H29" s="31">
         <v>43122</v>
@@ -4674,7 +4822,7 @@
     <row r="30" spans="3:13">
       <c r="C30" s="17"/>
       <c r="F30" s="34" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
@@ -4707,7 +4855,7 @@
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="M32" s="38">
         <v>50000000</v>
@@ -4722,7 +4870,7 @@
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="M33" s="38">
         <f>M30-M32</f>
@@ -4878,13 +5026,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12380952380952" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.12380952380952" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="25.8761904761905" customWidth="1"/>
     <col min="2" max="2" width="15.752380952381" style="17"/>
@@ -4892,24 +5040,24 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B2" s="18">
-        <v>48243101</v>
+        <v>47265212.64</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B3" s="17">
-        <f>-38000000+1100000</f>
-        <v>-36900000</v>
+        <f>-38000000</f>
+        <v>-38000000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="19" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B4" s="17">
         <v>-5000000</v>
@@ -4917,19 +5065,16 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B5" s="17">
-        <f>4300000+82000</f>
-        <v>4382000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <f>600000+700000+44000+1100000</f>
+        <v>2444000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="17">
-        <v>-1900000</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4942,29 +5087,33 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B9" s="17">
         <f>SUM(B2:B8)</f>
-        <v>29005101</v>
+        <v>26889212.64</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B10" s="17">
-        <f>'Mutasi Kas'!H84</f>
-        <v>27532000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <f>'Mutasi Kas'!H90</f>
+        <v>27357000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B12" s="17">
         <f>B9-B10</f>
-        <v>1473101</v>
+        <v>-467787.359999999</v>
+      </c>
+      <c r="D12" s="15" t="str">
+        <f>IF(B12&lt;0,"KURANG","LEBIH")</f>
+        <v>KURANG</v>
       </c>
     </row>
   </sheetData>
@@ -4999,13 +5148,13 @@
         <v>43121</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5026,7 +5175,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B3" s="13">
         <v>1000000</v>
@@ -5040,7 +5189,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="13" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B4" s="13">
         <v>400000</v>
@@ -5054,7 +5203,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="13" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B5" s="13">
         <v>1000000</v>
@@ -5068,7 +5217,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B6" s="13">
         <v>500000</v>
@@ -5076,7 +5225,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="13" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B7" s="13">
         <v>300000</v>
@@ -5084,7 +5233,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="13" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B8" s="13">
         <v>370000</v>
@@ -5092,7 +5241,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="13" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B9" s="13">
         <v>50000</v>
@@ -5100,7 +5249,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="13" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B10" s="13">
         <v>100000</v>
@@ -5108,7 +5257,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="13" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B11" s="13">
         <v>400000</v>
@@ -5116,7 +5265,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="13" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B12" s="13">
         <v>350000</v>
@@ -5124,7 +5273,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B13" s="13">
         <v>50000</v>
@@ -5137,7 +5286,7 @@
         <v>4520000</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E14" s="13">
         <f>SUM(E2:E13)</f>
@@ -5177,10 +5326,10 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="F1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5194,10 +5343,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>6</v>
@@ -5256,7 +5405,7 @@
         <v>10350000</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -5285,14 +5434,14 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B8" s="11">
         <f>SUM(B2:B7)</f>
         <v>34860000</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="H8" s="12">
         <f>B8-H5</f>
@@ -5302,7 +5451,7 @@
     <row r="9" spans="2:8">
       <c r="B9" s="6"/>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="H9" s="12">
         <v>3250000</v>
@@ -5311,7 +5460,7 @@
     <row r="10" spans="2:8">
       <c r="B10" s="6"/>
       <c r="E10" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H10" s="12">
         <f>H8-H9</f>
@@ -5377,7 +5526,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -5387,10 +5536,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5398,7 +5547,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C3" s="3">
         <f>7+12+11+17+17+13</f>
@@ -5410,7 +5559,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C4" s="3">
         <f>11+16+13+17+13+13+6+15</f>
@@ -5422,7 +5571,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C5" s="3">
         <f>12+14+16</f>
@@ -5434,7 +5583,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C6" s="3">
         <f>14+14+11+13+16+16</f>
@@ -5446,7 +5595,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C7" s="3">
         <f>5+8+13+3</f>
@@ -5458,7 +5607,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C8" s="3">
         <f>6+11+8+5</f>
@@ -5470,7 +5619,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C9" s="3">
         <v>14</v>
@@ -5478,7 +5627,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="3">
@@ -5488,7 +5637,7 @@
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C11">
         <f>C10*50000</f>
@@ -5497,7 +5646,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C13">
         <f>4+6+28+38+16+9+4+1</f>
@@ -5506,7 +5655,7 @@
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C14">
         <f>C13*100000</f>
@@ -5515,7 +5664,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C16">
         <f>C11+C14</f>

</xml_diff>